<commit_message>
REFACTOR: Finished Overlay Minor chang to Append/overlay
</commit_message>
<xml_diff>
--- a/QA/Tests/Running/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/Running/_Test_Suite_Statistics.xlsx
@@ -90,10 +90,10 @@
     <t>Automated</t>
   </si>
   <si>
-    <t>Inprogress</t>
-  </si>
-  <si>
-    <t>Needs History automation</t>
+    <t>Needs History automation to do the rest</t>
+  </si>
+  <si>
+    <t>Finished</t>
   </si>
 </sst>
 </file>
@@ -188,208 +188,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -765,7 +564,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,14 +601,14 @@
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -823,17 +622,17 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="6">
         <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -841,13 +640,13 @@
         <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
@@ -870,7 +669,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -891,7 +690,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -912,7 +711,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>7.2727272727272724E-2</v>
+        <v>0.18518518518518517</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -979,13 +778,13 @@
         <v>19</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1003,28 +802,28 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="31" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="3" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="2" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="1" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+    <cfRule type="containsText" dxfId="0" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
       <formula>NOT(ISERROR(SEARCH("Suited to Manual",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FUNCTIONALITY: Wrote a new test suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/Running/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/Running/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Title</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>NestedFolders</t>
+  </si>
+  <si>
+    <t>AllowImportPermissions</t>
+  </si>
+  <si>
+    <t>Uses User Permissions.</t>
   </si>
 </sst>
 </file>
@@ -191,7 +197,141 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -567,7 +707,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +737,7 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) -1</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -616,19 +756,19 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -640,53 +780,56 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
@@ -698,48 +841,48 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.19642857142857142</v>
+        <v>0.18333333333333332</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>20</v>
@@ -747,60 +890,74 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -818,30 +975,56 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+  <conditionalFormatting sqref="D1 D3:D1048576">
+    <cfRule type="containsText" dxfId="23" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="22" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="21" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="20" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="19" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="18" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="17" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+    <cfRule type="containsText" dxfId="16" priority="16" stopIfTrue="1" operator="containsText" text="Suited to Manual">
       <formula>NOT(ISERROR(SEARCH("Suited to Manual",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="15" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+      <formula>NOT(ISERROR(SEARCH("Suited to Manual",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: AllowImportPermissions - Wrote a new test case. Read - Updated existing test cases.
</commit_message>
<xml_diff>
--- a/QA/Tests/Running/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/Running/_Test_Suite_Statistics.xlsx
@@ -640,7 +640,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>22</v>
@@ -748,7 +748,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.25806451612903225</v>
+        <v>0.25396825396825395</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FUNCTIONALITY: updated stats moved manager path tests into Nested Folders
</commit_message>
<xml_diff>
--- a/QA/Tests/Running/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/Running/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Title</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Uses User Permissions.</t>
-  </si>
-  <si>
-    <t>ManagerPaths</t>
   </si>
 </sst>
 </file>
@@ -197,141 +194,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -774,7 +637,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,21 +667,21 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) -1</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -885,7 +748,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -906,7 +769,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -927,7 +790,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.41666666666666669</v>
+        <v>0.47457627118644069</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -974,27 +837,27 @@
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>22</v>
@@ -1002,43 +865,29 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1">
-        <v>4</v>
-      </c>
-      <c r="D14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1056,82 +905,56 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D1 D3:D9 D11:D1048576">
-    <cfRule type="containsText" dxfId="31" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
+  <conditionalFormatting sqref="D1 D15:D1048576 D3:D13">
+    <cfRule type="containsText" dxfId="15" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="14" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="13" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="12" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="11" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="10" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="9" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+    <cfRule type="containsText" dxfId="8" priority="24" stopIfTrue="1" operator="containsText" text="Suited to Manual">
       <formula>NOT(ISERROR(SEARCH("Suited to Manual",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="23" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="7" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="6" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="5" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="4" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="3" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="2" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="1" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="16" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+    <cfRule type="containsText" dxfId="0" priority="16" stopIfTrue="1" operator="containsText" text="Suited to Manual">
       <formula>NOT(ISERROR(SEARCH("Suited to Manual",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="containsText" dxfId="15" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
-      <formula>NOT(ISERROR(SEARCH("Suited to Manual",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Re-wrote the test suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/Running/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/Running/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Title</t>
   </si>
@@ -111,7 +111,7 @@
     <t>NativeFiles</t>
   </si>
   <si>
-    <t>in progress</t>
+    <t>Complicated</t>
   </si>
 </sst>
 </file>
@@ -206,7 +206,141 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -716,7 +850,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,7 +961,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -872,7 +1006,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.46575342465753422</v>
+        <v>0.45333333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -953,9 +1087,12 @@
         <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1016,81 +1153,107 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="D1 D3:D5 D7:D11 D13:D1048576">
-    <cfRule type="containsText" dxfId="23" priority="25" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="39" priority="33" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="38" priority="34" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="27" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="37" priority="35" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="28" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="36" priority="36" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="29" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="35" priority="37" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="30" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="34" priority="38" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="31" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="33" priority="39" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="32" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+    <cfRule type="containsText" dxfId="32" priority="40" stopIfTrue="1" operator="containsText" text="Suited to Manual">
       <formula>NOT(ISERROR(SEARCH("Suited to Manual",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="15" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="31" priority="25" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="30" priority="26" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="29" priority="27" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="28" priority="28" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="27" priority="29" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="26" priority="30" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="25" priority="31" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="24" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+    <cfRule type="containsText" dxfId="24" priority="32" stopIfTrue="1" operator="containsText" text="Suited to Manual">
       <formula>NOT(ISERROR(SEARCH("Suited to Manual",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="23" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="22" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="21" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="20" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="19" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="18" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="17" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+    <cfRule type="containsText" dxfId="16" priority="16" stopIfTrue="1" operator="containsText" text="Suited to Manual">
       <formula>NOT(ISERROR(SEARCH("Suited to Manual",D6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="containsText" dxfId="15" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+      <formula>NOT(ISERROR(SEARCH("Suited to Manual",D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Corrected a test suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/Running/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/Running/_Test_Suite_Statistics.xlsx
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>